<commit_message>
Added Cultervirus reference sequence
</commit_message>
<xml_diff>
--- a/tabular/core/borna-ncbi-refseqs-side-data.xlsx
+++ b/tabular/core/borna-ncbi-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA-ve/Bornaviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49843C64-8498-4142-BB6B-7E33CE0E5D85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09841267-7455-BD40-8B92-B1649A4CF04A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26620" yWindow="2220" windowWidth="21840" windowHeight="13240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5480" yWindow="2360" windowWidth="21840" windowHeight="13240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flavi.txt" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
   <si>
     <t>Alkhumra hemorrhagic fever virus</t>
   </si>
@@ -245,6 +245,18 @@
   </si>
   <si>
     <t>Carbovirus</t>
+  </si>
+  <si>
+    <t>MG599939</t>
+  </si>
+  <si>
+    <t>WSBV</t>
+  </si>
+  <si>
+    <t>Wuhan sharpbelly bornavirus</t>
+  </si>
+  <si>
+    <t>Cultervirus</t>
   </si>
 </sst>
 </file>
@@ -2195,11 +2207,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCellId="3" sqref="A13:F16 E12:F12 A12:C12 A1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2506,6 +2518,24 @@
         <v>71</v>
       </c>
       <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="15"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">

</xml_diff>